<commit_message>
http json mobile task
</commit_message>
<xml_diff>
--- a/industrial-java/task6/Document.xlsx
+++ b/industrial-java/task6/Document.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Авансовый отчет</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>fsdfsd - fsfd</t>
+  </si>
+  <si>
+    <t>Надо было</t>
+  </si>
+  <si>
+    <t>12.12.2022 - 24.12.2022</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -499,7 +505,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -515,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -523,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>324234.0</v>
+        <v>100000.0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -545,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>234324.0</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -553,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>324.0</v>
+        <v>60000.0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -561,7 +567,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>4234.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -569,7 +575,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>238882.0</v>
+        <v>85000.0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -577,7 +583,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>85352.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>